<commit_message>
fixing normal range for T
</commit_message>
<xml_diff>
--- a/notebooks/CYP21A2/input/CYP21A2_Xu_2019.xlsx
+++ b/notebooks/CYP21A2/input/CYP21A2_Xu_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/GIT/phenopacket-store/notebooks/CYP21A2/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959987DE-EFD8-E749-BC33-5581604D28D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A3EBD8-BB03-004C-87BF-E1040A690C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{BA0983D7-D97B-184B-858E-3667AA9A1415}"/>
+    <workbookView xWindow="12480" yWindow="1600" windowWidth="38400" windowHeight="19640" xr2:uid="{BA0983D7-D97B-184B-858E-3667AA9A1415}"/>
   </bookViews>
   <sheets>
     <sheet name="mydata" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="475">
   <si>
     <t>individual</t>
   </si>
@@ -1263,9 +1263,6 @@
   </si>
   <si>
     <t>P2M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1M </t>
   </si>
   <si>
     <t>P20Y</t>
@@ -2365,7 +2362,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2390,22 +2387,22 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>438</v>
+      </c>
+      <c r="I1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J1" t="s">
+        <v>447</v>
+      </c>
+      <c r="K1" t="s">
         <v>439</v>
-      </c>
-      <c r="I1" t="s">
-        <v>447</v>
-      </c>
-      <c r="J1" t="s">
-        <v>448</v>
-      </c>
-      <c r="K1" t="s">
-        <v>440</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
@@ -2417,28 +2414,28 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
+        <v>431</v>
+      </c>
+      <c r="P1" t="s">
         <v>432</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>433</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>434</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>474</v>
+      </c>
+      <c r="T1" t="s">
         <v>435</v>
       </c>
-      <c r="S1" t="s">
-        <v>475</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>436</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>437</v>
-      </c>
-      <c r="V1" t="s">
-        <v>438</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>372</v>
@@ -2506,7 +2503,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -2533,19 +2530,19 @@
         <v>10</v>
       </c>
       <c r="O2" t="s">
+        <v>472</v>
+      </c>
+      <c r="P2" t="s">
         <v>473</v>
       </c>
-      <c r="P2" t="s">
-        <v>474</v>
-      </c>
       <c r="Q2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="R2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="S2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T2" t="s">
         <v>11</v>
@@ -2631,7 +2628,7 @@
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -2747,7 +2744,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
@@ -2860,10 +2857,10 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
@@ -2979,7 +2976,7 @@
         <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J6" t="s">
         <v>43</v>
@@ -3095,7 +3092,7 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J7" t="s">
         <v>51</v>
@@ -3324,10 +3321,10 @@
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J9" t="s">
         <v>65</v>
@@ -3443,7 +3440,7 @@
         <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J10" t="s">
         <v>72</v>
@@ -3559,7 +3556,7 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J11" t="s">
         <v>19</v>
@@ -3675,7 +3672,7 @@
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J12" t="s">
         <v>19</v>
@@ -3788,13 +3785,13 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K13" t="s">
         <v>87</v>
@@ -3907,7 +3904,7 @@
         <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J14" t="s">
         <v>19</v>
@@ -4020,13 +4017,13 @@
         <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I15" t="s">
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K15" t="s">
         <v>97</v>
@@ -4121,7 +4118,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D16">
         <v>815.2</v>
@@ -4136,13 +4133,13 @@
         <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K16" t="s">
         <v>102</v>
@@ -4237,7 +4234,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D17">
         <v>238.9</v>
@@ -4252,13 +4249,13 @@
         <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K17" t="s">
         <v>97</v>
@@ -4368,13 +4365,13 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K18" t="s">
         <v>97</v>
@@ -4469,7 +4466,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D19">
         <v>824</v>
@@ -4484,13 +4481,13 @@
         <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K19" t="s">
         <v>97</v>
@@ -4585,7 +4582,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D20">
         <v>535</v>
@@ -4600,13 +4597,13 @@
         <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I20" t="s">
         <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K20" t="s">
         <v>97</v>
@@ -4701,7 +4698,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D21">
         <v>351</v>
@@ -4716,10 +4713,10 @@
         <v>18</v>
       </c>
       <c r="H21" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I21" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J21" t="s">
         <v>96</v>
@@ -4832,10 +4829,10 @@
         <v>18</v>
       </c>
       <c r="H22" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I22" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J22" t="s">
         <v>96</v>
@@ -4933,7 +4930,7 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D23">
         <v>328</v>
@@ -4948,10 +4945,10 @@
         <v>18</v>
       </c>
       <c r="H23" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I23" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J23" t="s">
         <v>96</v>
@@ -5049,7 +5046,7 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
@@ -5064,10 +5061,10 @@
         <v>18</v>
       </c>
       <c r="H24" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I24" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J24" t="s">
         <v>96</v>
@@ -5180,10 +5177,10 @@
         <v>18</v>
       </c>
       <c r="H25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J25" t="s">
         <v>96</v>
@@ -5296,7 +5293,7 @@
         <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I26" t="s">
         <v>43</v>
@@ -5412,7 +5409,7 @@
         <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I27" t="s">
         <v>19</v>
@@ -5528,7 +5525,7 @@
         <v>18</v>
       </c>
       <c r="H28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I28" t="s">
         <v>43</v>
@@ -5644,7 +5641,7 @@
         <v>18</v>
       </c>
       <c r="H29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I29" t="s">
         <v>19</v>
@@ -5760,10 +5757,10 @@
         <v>18</v>
       </c>
       <c r="H30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J30" t="s">
         <v>96</v>
@@ -5876,10 +5873,10 @@
         <v>18</v>
       </c>
       <c r="H31" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J31" t="s">
         <v>96</v>
@@ -5992,10 +5989,10 @@
         <v>18</v>
       </c>
       <c r="H32" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J32" t="s">
         <v>96</v>
@@ -6108,7 +6105,7 @@
         <v>18</v>
       </c>
       <c r="H33" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I33" t="s">
         <v>19</v>
@@ -6224,10 +6221,10 @@
         <v>18</v>
       </c>
       <c r="H34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J34" t="s">
         <v>96</v>
@@ -6340,10 +6337,10 @@
         <v>18</v>
       </c>
       <c r="H35" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I35" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J35" t="s">
         <v>96</v>
@@ -6456,7 +6453,7 @@
         <v>18</v>
       </c>
       <c r="H36" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I36" t="s">
         <v>19</v>
@@ -6557,7 +6554,7 @@
         <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D37">
         <v>246.4</v>
@@ -6572,10 +6569,10 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I37" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J37" t="s">
         <v>96</v>
@@ -6673,7 +6670,7 @@
         <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D38">
         <v>329.7</v>
@@ -6688,10 +6685,10 @@
         <v>18</v>
       </c>
       <c r="H38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J38" t="s">
         <v>96</v>
@@ -6804,10 +6801,10 @@
         <v>18</v>
       </c>
       <c r="H39" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I39" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J39" t="s">
         <v>96</v>
@@ -6905,7 +6902,7 @@
         <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D40" t="s">
         <v>18</v>
@@ -6920,7 +6917,7 @@
         <v>18</v>
       </c>
       <c r="H40" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I40" t="s">
         <v>43</v>
@@ -7039,7 +7036,7 @@
         <v>214</v>
       </c>
       <c r="I41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J41" t="s">
         <v>214</v>
@@ -7155,7 +7152,7 @@
         <v>222</v>
       </c>
       <c r="I42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J42" t="s">
         <v>222</v>
@@ -7271,7 +7268,7 @@
         <v>222</v>
       </c>
       <c r="I43" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J43" t="s">
         <v>222</v>
@@ -7369,7 +7366,7 @@
         <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -7381,13 +7378,13 @@
         <v>555</v>
       </c>
       <c r="G44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H44" t="s">
         <v>222</v>
       </c>
       <c r="I44" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J44" t="s">
         <v>222</v>
@@ -7417,13 +7414,13 @@
         <v>48.93</v>
       </c>
       <c r="S44" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T44" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="U44" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="V44" t="s">
         <v>18</v>
@@ -7485,7 +7482,7 @@
         <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D45">
         <v>87.5</v>
@@ -7503,7 +7500,7 @@
         <v>214</v>
       </c>
       <c r="I45" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J45" t="s">
         <v>214</v>
@@ -7601,7 +7598,7 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D46">
         <v>93.4</v>
@@ -7619,7 +7616,7 @@
         <v>214</v>
       </c>
       <c r="I46" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J46" t="s">
         <v>214</v>
@@ -7649,13 +7646,13 @@
         <v>40.369999999999997</v>
       </c>
       <c r="S46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T46" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="U46" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="V46" t="s">
         <v>18</v>
@@ -7717,7 +7714,7 @@
         <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D47">
         <v>158.4</v>
@@ -7735,7 +7732,7 @@
         <v>214</v>
       </c>
       <c r="I47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J47" t="s">
         <v>214</v>
@@ -7851,7 +7848,7 @@
         <v>214</v>
       </c>
       <c r="I48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J48" t="s">
         <v>214</v>
@@ -7949,7 +7946,7 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D49" t="s">
         <v>18</v>
@@ -8083,7 +8080,7 @@
         <v>214</v>
       </c>
       <c r="I50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J50" t="s">
         <v>214</v>
@@ -8175,13 +8172,13 @@
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B51" t="s">
         <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D51">
         <v>168.8</v>
@@ -8294,7 +8291,7 @@
         <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -8404,13 +8401,13 @@
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B53" t="s">
         <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -8428,13 +8425,13 @@
         <v>214</v>
       </c>
       <c r="I53" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L53" t="s">
         <v>21</v>
@@ -8520,7 +8517,7 @@
         <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D54">
         <v>217</v>
@@ -8868,7 +8865,7 @@
         <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D57" t="s">
         <v>18</v>
@@ -8883,10 +8880,10 @@
         <v>18</v>
       </c>
       <c r="H57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I57" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J57" t="s">
         <v>288</v>
@@ -9002,13 +8999,13 @@
         <v>308</v>
       </c>
       <c r="I58" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J58" t="s">
         <v>297</v>
       </c>
       <c r="K58" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L58" t="s">
         <v>290</v>
@@ -9234,7 +9231,7 @@
         <v>308</v>
       </c>
       <c r="I60" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J60" t="s">
         <v>308</v>
@@ -9347,13 +9344,13 @@
         <v>18</v>
       </c>
       <c r="H61" t="s">
+        <v>468</v>
+      </c>
+      <c r="I61" t="s">
         <v>469</v>
       </c>
-      <c r="I61" t="s">
-        <v>470</v>
-      </c>
       <c r="J61" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K61" t="s">
         <v>316</v>
@@ -9448,7 +9445,7 @@
         <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D62">
         <v>87.5</v>
@@ -9466,7 +9463,7 @@
         <v>322</v>
       </c>
       <c r="I62" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J62" t="s">
         <v>322</v>
@@ -9564,7 +9561,7 @@
         <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D63">
         <v>25</v>
@@ -9582,7 +9579,7 @@
         <v>288</v>
       </c>
       <c r="I63" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J63" t="s">
         <v>288</v>
@@ -9680,7 +9677,7 @@
         <v>69</v>
       </c>
       <c r="C64" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D64">
         <v>27.3</v>
@@ -9698,7 +9695,7 @@
         <v>308</v>
       </c>
       <c r="I64" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J64" t="s">
         <v>308</v>
@@ -9811,7 +9808,7 @@
         <v>18</v>
       </c>
       <c r="H65" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I65" t="s">
         <v>214</v>
@@ -9912,7 +9909,7 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D66">
         <v>31.4</v>
@@ -9930,7 +9927,7 @@
         <v>343</v>
       </c>
       <c r="I66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J66" t="s">
         <v>343</v>
@@ -10043,10 +10040,10 @@
         <v>18</v>
       </c>
       <c r="H67" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I67" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J67" t="s">
         <v>349</v>
@@ -10159,13 +10156,13 @@
         <v>18</v>
       </c>
       <c r="H68" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I68" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J68" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K68" t="s">
         <v>355</v>
@@ -10272,10 +10269,10 @@
         <v>18</v>
       </c>
       <c r="H69" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J69" t="s">
         <v>358</v>
@@ -10388,10 +10385,10 @@
         <v>18</v>
       </c>
       <c r="H70" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I70" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J70" t="s">
         <v>364</v>
@@ -10504,13 +10501,13 @@
         <v>18</v>
       </c>
       <c r="H71" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I71" t="s">
         <v>214</v>
       </c>
       <c r="J71" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K71" t="s">
         <v>370</v>

</xml_diff>